<commit_message>
feat: phase2.1 ops maturity implementation (PR1-PR3) with evidence and docs
</commit_message>
<xml_diff>
--- a/docs/references/CS_AI_CHATBOT_DB.xlsx
+++ b/docs/references/CS_AI_CHATBOT_DB.xlsx
@@ -71,6 +71,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TB_COST_RATE_CARD" sheetId="62" state="visible" r:id="rId62"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TB_RBAC_MATRIX" sheetId="63" state="visible" r:id="rId63"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TB_OPS_BLOCK" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TB_AUDIT_EXPORT_JOB" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TB_AUDIT_EXPORT_CHUNK" sheetId="66" state="visible" r:id="rId66"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TB_SCHEDULER_LOCK" sheetId="67" state="visible" r:id="rId67"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'목차'!$A$7:$D$68</definedName>
@@ -1038,7 +1041,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
@@ -1071,7 +1074,7 @@
     <row r="3" ht="21" customHeight="1">
       <c r="A3" s="15" t="inlineStr">
         <is>
-          <t>작성일: 2026-02-17</t>
+          <t>???: 2026-02-21</t>
         </is>
       </c>
       <c r="B3" s="15" t="n"/>
@@ -1081,7 +1084,7 @@
     <row r="4" ht="21" customHeight="1">
       <c r="A4" s="15" t="inlineStr">
         <is>
-          <t>총 테이블: 61개</t>
+          <t>? ???: 66?</t>
         </is>
       </c>
       <c r="B4" s="15" t="n"/>
@@ -1091,7 +1094,7 @@
     <row r="5" ht="21" customHeight="1">
       <c r="A5" s="16" t="inlineStr">
         <is>
-          <t>그룹별: AI 설정/정책 13개, Billing/Quota 6개, Ops/Observability 1개, RAG/안전 5개, VectorOps 1개, 공통 2개, 권한/테넌트 10개, 운영/감사 7개, 지식베이스 8개, 채팅/상담 8개</t>
+          <t>??? ??? ?? ?? ???? ?? ?? ??(?? ?? ??)</t>
         </is>
       </c>
       <c r="B5" s="16" t="n"/>
@@ -2344,6 +2347,106 @@
       <c r="D68" s="69" t="inlineStr">
         <is>
           <t>Billing/Quota</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>62</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>TB_RBAC_MATRIX</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>TB_RBAC_MATRIX</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>63</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>TB_OPS_BLOCK</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>TB_OPS_BLOCK</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>??/??</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>64</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>TB_AUDIT_EXPORT_JOB</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>TB_AUDIT_EXPORT_JOB</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>??/??</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>65</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>TB_AUDIT_EXPORT_CHUNK</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>TB_AUDIT_EXPORT_CHUNK</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>??/??</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>66</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>TB_SCHEDULER_LOCK</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>TB_SCHEDULER_LOCK</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>??/??</t>
         </is>
       </c>
     </row>
@@ -23325,6 +23428,1195 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TB_AUDIT_EXPORT_JOB - table specification</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>?????</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>KEY</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Export job ID</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>V7 async export spool</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>tenant_id</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>FK</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Tenant ID</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>FK -&gt; TB_TENANT.id</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>requested_by</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Requested user ID</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>varchar(20)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Job status</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>PENDING/RUNNING/DONE/FAILED/EXPIRED</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>export_format</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>varchar(20)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>json</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Export format</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>json|csv</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>from_utc</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Range start UTC</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>to_utc</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Range end UTC</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>row_limit</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Row limit</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>tenant/date/row guardrail</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>max_bytes</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5242880</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Max payload bytes</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>max_duration_sec</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Max processing duration(sec)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>row_count</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Exported row count</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>total_bytes</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Exported total bytes</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>error_code</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>varchar(80)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Failure code</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>error_message</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>varchar(500)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Failure detail</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>expires_at</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Payload expiry UTC</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>default TTL 24h</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>trace_id</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Trace ID</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>trace linkage mandatory</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CURRENT_TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Created at UTC</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>started_at</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Worker started at UTC</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>completed_at</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Completed at UTC</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TB_AUDIT_EXPORT_CHUNK - table specification</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>?????</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>KEY</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>job_id</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PK/FK</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Export job ID</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>FK -&gt; TB_AUDIT_EXPORT_JOB.id, ON DELETE CASCADE</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>chunk_no</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>integer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Chunk order</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>payload_bytes</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>bytea</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Chunk payload bytes</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>sanitized payload only</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>payload_hash</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>varchar(128)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Chunk SHA-256</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CURRENT_TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Created at UTC</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TB_SCHEDULER_LOCK - table specification</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>?????</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>KEY</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>??</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>lock_key</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>varchar(120)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Scheduler lock key</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>owner_id</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Lock owner instance ID</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>lease_until_utc</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Lease expiration UTC</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>fencing_token</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>bigint</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Fencing token</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>monotonic</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>last_heartbeat_utc</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Last heartbeat UTC</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>V8 self-healing</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>last_recovered_at</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Last recovery UTC</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>V8 self-healing</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>recovery_count</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>bigint</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Recovery count</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>V8 self-healing</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NOT NULL</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CURRENT_TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Updated at UTC</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>